<commit_message>
Read and write txt file with python
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -509,80 +509,80 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>코로나 신규 확진자 63명…추석 연휴 이후가 변곡점</t>
+          <t>추석연휴 제주 관광객 20만명 넘었다…제주공항 북적</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://www.hani.co.kr/arti/society/health/964213.html</t>
+          <t>http://www.wowtv.co.kr/NewsCenter/News/Read?articleId=A202010020048&amp;t=NN</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>한겨레</t>
+          <t>한국경제TV</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>구름 사이 '휘영청' 추석 보름달, 가장 높게 뜨는 시각은?</t>
+          <t>추석인데…모자간에 남매간에 잇단 칼부림 '비극'(종합)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://biz.chosun.com/site/data/html_dir/2020/10/01/2020100100136.html?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=biz</t>
+          <t>http://news.tf.co.kr/read/national/1816181.htm</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>조선비즈</t>
+          <t>더팩트</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>이낙연 대표, 추석 맞아 고 노무현 대통령 묘소 참배</t>
+          <t>구름 사이 '휘영청' 추석 보름달, 가장 높게 뜨는 시각은?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://imnews.imbc.com/news/2020/politics/article/5927450_32626.html</t>
+          <t>https://biz.chosun.com/site/data/html_dir/2020/10/01/2020100100136.html?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=biz</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MBC</t>
+          <t>조선비즈</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>추미애·조국, 추석날 주거니받거니 “일부 정치검찰 정권과 결탁”</t>
+          <t>소시지 3개에 김치 3조각... 격리된 병사가 먹은 추석날 저녁</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.chosun.com/national/national_general/2020/10/01/7BNGFKXKWZELRL2OONEPG2TKCU/?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=news</t>
+          <t>http://www.ohmynews.com/NWS_Web/View/at_pg.aspx?CNTN_CD=A0002680782&amp;CMPT_CD=P0010&amp;utm_source=naver&amp;utm_medium=newsearch&amp;utm_campaign=naver_news</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>조선일보</t>
+          <t>오마이뉴스</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>'추석 특수' 누린 한우·삼겹살…소비자가격 고공행진</t>
+          <t>이낙연 대표, 추석 맞아 고 노무현 대통령 묘소 참배</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://imnews.imbc.com/news/2020/econo/article/5927149_32647.html</t>
+          <t>https://imnews.imbc.com/news/2020/politics/article/5927450_32626.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>추석날 고속도로 오후 1~2시 정체 극심…“오후 10시쯤 해소 전망”</t>
+          <t>추미애·조국, 추석날 주거니받거니 “일부 정치검찰 정권과 결탁”</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>http://news.kbs.co.kr/news/view.do?ncd=5016431&amp;ref=A</t>
+          <t>https://www.chosun.com/national/national_general/2020/10/01/7BNGFKXKWZELRL2OONEPG2TKCU/?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=news</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>KBS</t>
+          <t>조선일보</t>
         </is>
       </c>
     </row>

</xml_diff>